<commit_message>
- Updated files for small sound attenuating chamber.
</commit_message>
<xml_diff>
--- a/Sound_attenuating_chamber_small/sound_attenuating_chamber_BOM.xlsx
+++ b/Sound_attenuating_chamber_small/sound_attenuating_chamber_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Dropbox\Hardware development\pyControl_hardware\Sound_attenuating_chamber_small\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B61AF8E-7B3B-49EB-8150-F994A7A2C402}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF6C442-4B5A-4A01-9E6D-2E53C2026051}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="12735" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15912" yWindow="2880" windowWidth="13188" windowHeight="13644" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="87">
   <si>
     <t>Part</t>
   </si>
@@ -223,15 +223,9 @@
     <t>Point Grey</t>
   </si>
   <si>
-    <t>8mm CS mount Lens</t>
-  </si>
-  <si>
     <t>Computar</t>
   </si>
   <si>
-    <t>T0812FICS</t>
-  </si>
-  <si>
     <t>ACC-01-3013</t>
   </si>
   <si>
@@ -247,9 +241,6 @@
     <t>Chameleon  tripod adapter</t>
   </si>
   <si>
-    <t>https://www.amazon.co.uk/SIOTI-Head-Metal-Ballhead-Digital-Compact/dp/B071GQLJKZ/</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cap head bolt  1/4-20 UNC x 1" </t>
   </si>
   <si>
@@ -262,9 +253,6 @@
     <t>477-4878</t>
   </si>
   <si>
-    <t>Mini Ball head mount</t>
-  </si>
-  <si>
     <t>Chameleon USB3 cable</t>
   </si>
   <si>
@@ -278,13 +266,34 @@
   </si>
   <si>
     <t>176-6768</t>
+  </si>
+  <si>
+    <t>ACCU group</t>
+  </si>
+  <si>
+    <t>SSC-1/4-20-1-A2</t>
+  </si>
+  <si>
+    <t>T4Z2813CS-IR</t>
+  </si>
+  <si>
+    <t>2.8-12mm CS mount Lens</t>
+  </si>
+  <si>
+    <t>Ulanzi Mini Ball head mount</t>
+  </si>
+  <si>
+    <t>UL-U30</t>
+  </si>
+  <si>
+    <t>UK Digital</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -304,14 +313,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -343,11 +344,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -378,10 +378,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -662,29 +660,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="10.140625"/>
-    <col min="7" max="8" width="8.5703125"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
-    <col min="10" max="1026" width="8.5703125"/>
+    <col min="1" max="1" width="25.88671875" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="10.109375"/>
+    <col min="7" max="8" width="8.5546875"/>
+    <col min="9" max="9" width="16.109375" customWidth="1"/>
+    <col min="10" max="1026" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>37</v>
       </c>
       <c r="E1" s="9"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -696,7 +694,7 @@
       </c>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>37</v>
       </c>
@@ -707,13 +705,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E4" s="9"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>39</v>
       </c>
@@ -724,7 +722,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>43</v>
       </c>
@@ -735,7 +733,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>44</v>
       </c>
@@ -746,7 +744,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>45</v>
       </c>
@@ -757,7 +755,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>46</v>
       </c>
@@ -768,7 +766,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>0</v>
       </c>
@@ -782,7 +780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>47</v>
       </c>
@@ -796,7 +794,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>49</v>
       </c>
@@ -810,13 +808,13 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>51</v>
       </c>
       <c r="E14" s="9"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>59</v>
       </c>
@@ -830,18 +828,21 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>52</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="E16" s="10">
-        <v>2543656</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16">
+        <v>1924856</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>54</v>
       </c>
@@ -855,7 +856,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>56</v>
       </c>
@@ -869,7 +870,7 @@
         <v>359154</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>47</v>
       </c>
@@ -883,7 +884,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>57</v>
       </c>
@@ -897,15 +898,15 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>62</v>
       </c>
       <c r="E21" s="9"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -917,9 +918,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -928,12 +929,12 @@
         <v>64</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -942,12 +943,12 @@
         <v>64</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -956,54 +957,54 @@
         <v>64</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="E26" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
-      <c r="D27" s="14" t="s">
-        <v>73</v>
+      <c r="D27" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1012,12 +1013,12 @@
         <v>32</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1026,12 +1027,12 @@
         <v>32</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1040,16 +1041,16 @@
         <v>32</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E32" s="9"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="7" t="s">
         <v>21</v>
       </c>
@@ -1063,7 +1064,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>29</v>
       </c>
@@ -1077,7 +1078,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>24</v>
       </c>
@@ -1091,7 +1092,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>28</v>
       </c>
@@ -1105,7 +1106,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>27</v>
       </c>
@@ -1119,7 +1120,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>33</v>
       </c>
@@ -1133,7 +1134,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>34</v>
       </c>
@@ -1161,17 +1162,17 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1182,7 +1183,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1193,7 +1194,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1204,7 +1205,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1212,7 +1213,7 @@
         <v>1691</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1220,7 +1221,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1228,7 +1229,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1236,7 +1237,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1244,12 +1245,12 @@
         <v>622</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1257,7 +1258,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1265,12 +1266,12 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>

</xml_diff>